<commit_message>
***v1.12.2.4    2020/10/27  (Mark Chou) 功能修改 加入二期MTL,MTS,HID設定
</commit_message>
<xml_diff>
--- a/OverhaedHoistTransporter_CSOT/BCWinForm/Config/Taichung/CSTTranSchedule.xlsx
+++ b/OverhaedHoistTransporter_CSOT/BCWinForm/Config/Taichung/CSTTranSchedule.xlsx
@@ -341,41 +341,38 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F6"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="H4" sqref="H4:H5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1"/>
       <c r="B1" s="1">
-        <v>30103</v>
+        <v>20411</v>
       </c>
       <c r="C1" s="1">
-        <v>20311</v>
+        <v>20416</v>
       </c>
       <c r="D1">
         <v>20316</v>
       </c>
       <c r="E1">
-        <v>30101</v>
-      </c>
-      <c r="F1">
-        <v>20616</v>
+        <v>20611</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
-        <v>30103</v>
+        <v>20411</v>
       </c>
       <c r="B2">
         <v>0</v>
       </c>
       <c r="C2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D2">
         <v>1</v>
@@ -383,31 +380,25 @@
       <c r="E2">
         <v>1</v>
       </c>
-      <c r="F2">
-        <v>1</v>
-      </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
-        <v>20311</v>
+        <v>20416</v>
       </c>
       <c r="B3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="C3">
         <v>0</v>
       </c>
       <c r="D3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
-      <c r="F3">
-        <v>1</v>
-      </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>20316</v>
       </c>
@@ -415,21 +406,18 @@
         <v>1</v>
       </c>
       <c r="C4">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="D4">
         <v>0</v>
       </c>
       <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>30101</v>
+        <v>20611</v>
       </c>
       <c r="B5">
         <v>1</v>
@@ -438,32 +426,9 @@
         <v>1</v>
       </c>
       <c r="D5">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="E5">
-        <v>0</v>
-      </c>
-      <c r="F5">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A6">
-        <v>20616</v>
-      </c>
-      <c r="B6">
-        <v>1</v>
-      </c>
-      <c r="C6">
-        <v>1</v>
-      </c>
-      <c r="D6">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
         <v>0</v>
       </c>
     </row>

</xml_diff>